<commit_message>
?????? ??????????? + edit
</commit_message>
<xml_diff>
--- a/doc/������ �����������.xlsx
+++ b/doc/������ �����������.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950"/>
+    <workbookView xWindow="240" yWindow="168" windowWidth="14808" windowHeight="7956"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -66,17 +66,17 @@
     <t>3 диалога tutorials + research и некоторые иные properties</t>
   </si>
   <si>
-    <t>journal, help, gameover</t>
-  </si>
-  <si>
-    <t>private_messages</t>
+    <t xml:space="preserve">Папка crew </t>
+  </si>
+  <si>
+    <t>Journal, help, gameover, private_messages</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -114,7 +114,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -127,9 +127,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Стандартная">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -167,7 +167,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Стандартная">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -201,6 +201,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -235,9 +236,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Стандартная">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -410,22 +412,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="32" customWidth="1"/>
-    <col min="2" max="2" width="25.7109375" style="1" customWidth="1"/>
-    <col min="3" max="4" width="23.42578125" customWidth="1"/>
-    <col min="5" max="5" width="14.5703125" customWidth="1"/>
+    <col min="1" max="1" width="53.21875" customWidth="1"/>
+    <col min="2" max="2" width="25.6640625" style="1" customWidth="1"/>
+    <col min="3" max="4" width="23.44140625" customWidth="1"/>
+    <col min="5" max="5" width="14.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -442,7 +444,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -456,7 +458,7 @@
         <v>41843</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -470,7 +472,7 @@
         <v>41850</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -484,7 +486,7 @@
         <v>41863</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="75">
+    <row r="5" spans="1:5" ht="72" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>9</v>
       </c>
@@ -498,7 +500,7 @@
         <v>41943</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -509,7 +511,7 @@
         <v>41980</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -520,7 +522,7 @@
         <v>41980</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -534,7 +536,7 @@
         <v>41987</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>14</v>
       </c>
@@ -548,29 +550,29 @@
         <v>41990</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>15</v>
       </c>
       <c r="B12" s="1">
-        <v>49</v>
+        <v>55.4</v>
       </c>
       <c r="D12">
-        <v>3430</v>
+        <v>3877</v>
       </c>
       <c r="E12" s="2">
-        <v>42002</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5">
+        <v>41983</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>16</v>
       </c>
       <c r="B13" s="1">
-        <v>18</v>
+        <v>67</v>
       </c>
       <c r="D13">
-        <v>1260</v>
+        <v>4690</v>
       </c>
       <c r="E13" s="2">
         <v>42002</v>
@@ -583,24 +585,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>